<commit_message>
0511 study and update
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" tabRatio="500" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,12 @@
     <sheet name="工作表4" sheetId="4" r:id="rId4"/>
     <sheet name="工作表5" sheetId="5" r:id="rId5"/>
     <sheet name="工作表6" sheetId="6" r:id="rId6"/>
+    <sheet name="工作表7" sheetId="7" r:id="rId7"/>
+    <sheet name="工作表8" sheetId="8" r:id="rId8"/>
+    <sheet name="工作表9" sheetId="9" r:id="rId9"/>
+    <sheet name="工作表10" sheetId="10" r:id="rId10"/>
+    <sheet name="工作表11" sheetId="11" r:id="rId11"/>
+    <sheet name="工作表12" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -32,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="58">
   <si>
     <t>编号</t>
     <rPh sb="0" eb="1">
@@ -250,6 +256,108 @@
     <rPh sb="0" eb="1">
       <t>lian'shu</t>
     </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>姓名</t>
+    <rPh sb="0" eb="1">
+      <t>xing'm</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学号</t>
+    <rPh sb="0" eb="1">
+      <t>xue'hao</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>成绩</t>
+    <rPh sb="0" eb="1">
+      <t>cheng'ji</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>名次</t>
+    <rPh sb="0" eb="1">
+      <t>ming'ci</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>张</t>
+    <rPh sb="0" eb="1">
+      <t>zhang</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>王</t>
+    <rPh sb="0" eb="1">
+      <t>wang</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>李</t>
+    <rPh sb="0" eb="1">
+      <t>li</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>赵</t>
+    <rPh sb="0" eb="1">
+      <t>zhao</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>班级</t>
+    <rPh sb="0" eb="1">
+      <t>ban'ji</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一班</t>
+    <rPh sb="0" eb="1">
+      <t>yi'ban</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>二班</t>
+    <rPh sb="0" eb="1">
+      <t>er'ban</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>三班</t>
+    <rPh sb="0" eb="1">
+      <t>san'ban</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f_成绩</t>
+    <rPh sb="2" eb="3">
+      <t>cheng'ji</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>e_成绩</t>
+    <rPh sb="2" eb="3">
+      <t>cheng'ji</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -309,8 +417,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -325,14 +445,26 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="19">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="18" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -706,6 +838,248 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3">
+        <v>101</v>
+      </c>
+      <c r="C3">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4">
+        <v>102</v>
+      </c>
+      <c r="C4">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5">
+        <v>103</v>
+      </c>
+      <c r="C5">
+        <v>550</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>100</v>
+      </c>
+      <c r="B2">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>100</v>
+      </c>
+      <c r="B3">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>101</v>
+      </c>
+      <c r="B4">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>101</v>
+      </c>
+      <c r="B5">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>102</v>
+      </c>
+      <c r="B6">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>102</v>
+      </c>
+      <c r="B7">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>103</v>
+      </c>
+      <c r="B8">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>103</v>
+      </c>
+      <c r="B9">
+        <v>650</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+      <c r="C3">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4">
+        <v>101</v>
+      </c>
+      <c r="C4">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5">
+        <v>102</v>
+      </c>
+      <c r="C5">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6">
+        <v>102</v>
+      </c>
+      <c r="C6">
+        <v>459</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
@@ -1147,7 +1521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -1237,4 +1611,233 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3">
+        <v>101</v>
+      </c>
+      <c r="D3">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4">
+        <v>102</v>
+      </c>
+      <c r="D4">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5">
+        <v>103</v>
+      </c>
+      <c r="D5">
+        <v>550</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>101</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>102</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>103</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="4" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5">
+        <v>100</v>
+      </c>
+      <c r="F5">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6">
+        <v>101</v>
+      </c>
+      <c r="F6">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7">
+        <v>102</v>
+      </c>
+      <c r="F7">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8">
+        <v>103</v>
+      </c>
+      <c r="F8">
+        <v>550</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>